<commit_message>
Updated to reflect gg becoming Maple
Updated to reflect gg becoming Maple. Includes vision and new scenerios
in notes doc and data models in visio
</commit_message>
<xml_diff>
--- a/ba/GeoGab notes.xlsx
+++ b/ba/GeoGab notes.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\e354ba7bf8.testurl.ws\ba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\GitHub\geogab\ba\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Menu-options" sheetId="3" r:id="rId2"/>
     <sheet name="NFRs" sheetId="4" r:id="rId3"/>
     <sheet name="Zoom-layering" sheetId="2" r:id="rId4"/>
+    <sheet name="Vision" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="95">
   <si>
     <t>Multilayered</t>
   </si>
@@ -270,6 +272,51 @@
   </si>
   <si>
     <t>The system shall support 1000 concurrent users</t>
+  </si>
+  <si>
+    <t>Why do we undervalue a map. We are most lively not going to travel to the other side of the city to visit a city. Especillay in a city like London has a good distribution of great places</t>
+  </si>
+  <si>
+    <t>Location centric approach to interacting with a city indivudualy, with friends or with trusted people and groups</t>
+  </si>
+  <si>
+    <t>A platform for the consolidation of map based content</t>
+  </si>
+  <si>
+    <t>Romantics</t>
+  </si>
+  <si>
+    <t>Jenny is in love and wants to record location of her and Steve's dates</t>
+  </si>
+  <si>
+    <t>Create a map which will be shared between them and calls it "Steve's and Jenny's love trail"</t>
+  </si>
+  <si>
+    <t>Steve doesn't have to approve the request like in whatsapp</t>
+  </si>
+  <si>
+    <t>Simple step</t>
+  </si>
+  <si>
+    <t>Detailed step</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Does looking for these venues imply a search and rich content on those places</t>
+  </si>
+  <si>
+    <t>Jenny starts to adding the dance club which they first met, the coffee shop they went on a date. The first restaurant and their second date which was a picnic at the top of primrose hill</t>
+  </si>
+  <si>
+    <t>She then want to add a layer of their favourite pubs</t>
+  </si>
+  <si>
+    <t>Steve thinks that Jenny has the location of the picnic incorrect it was in fact at Hamstead heath. Steve correct this</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steve is informed that there is a map that they both share. </t>
   </si>
 </sst>
 </file>
@@ -301,7 +348,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +376,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -389,6 +442,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,7 +963,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12:D13"/>
     </sheetView>
   </sheetViews>
@@ -1324,4 +1381,109 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="80.7109375" customWidth="1"/>
+    <col min="3" max="3" width="74.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="41" customWidth="1"/>
+    <col min="3" max="3" width="84.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" style="5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>